<commit_message>
updated the comprehensive table
</commit_message>
<xml_diff>
--- a/Notebooks/Comprehensive_Etsy_Store_Data.xlsx
+++ b/Notebooks/Comprehensive_Etsy_Store_Data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:DR1"/>
+  <dimension ref="A1:ES1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -531,517 +531,652 @@
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
+          <t>Total Items Left in Inventory Item 1</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
           <t>Item Sold 2 (with Reviews)</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>Title Item 2</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>Description Item 2</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>Price Item 2</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>Item Details 2</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>Ships From Item 2</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>Etsy POS Item Link 2</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>Reviews Item 2</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>Total Items Left in Inventory Item 2</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>Item Sold 3 (with Reviews)</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>Title Item 3</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>Description Item 3</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>Price Item 3</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>Item Details 3</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>Ships From Item 3</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>Etsy POS Item Link 3</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>Reviews Item 3</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>Total Items Left in Inventory Item 3</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>Item Sold 4 (with Reviews)</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>Title Item 4</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>Description Item 4</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>Price Item 4</t>
         </is>
       </c>
-      <c r="AN1" s="1" t="inlineStr">
+      <c r="AQ1" s="1" t="inlineStr">
         <is>
           <t>Item Details 4</t>
         </is>
       </c>
-      <c r="AO1" s="1" t="inlineStr">
+      <c r="AR1" s="1" t="inlineStr">
         <is>
           <t>Ships From Item 4</t>
         </is>
       </c>
-      <c r="AP1" s="1" t="inlineStr">
+      <c r="AS1" s="1" t="inlineStr">
         <is>
           <t>Etsy POS Item Link 4</t>
         </is>
       </c>
-      <c r="AQ1" s="1" t="inlineStr">
+      <c r="AT1" s="1" t="inlineStr">
         <is>
           <t>Reviews Item 4</t>
         </is>
       </c>
-      <c r="AR1" s="1" t="inlineStr">
+      <c r="AU1" s="1" t="inlineStr">
+        <is>
+          <t>Total Items Left in Inventory Item 4</t>
+        </is>
+      </c>
+      <c r="AV1" s="1" t="inlineStr">
         <is>
           <t>Item Sold 5 (with Reviews)</t>
         </is>
       </c>
-      <c r="AS1" s="1" t="inlineStr">
+      <c r="AW1" s="1" t="inlineStr">
         <is>
           <t>Title Item 5</t>
         </is>
       </c>
-      <c r="AT1" s="1" t="inlineStr">
+      <c r="AX1" s="1" t="inlineStr">
         <is>
           <t>Description Item 5</t>
         </is>
       </c>
-      <c r="AU1" s="1" t="inlineStr">
+      <c r="AY1" s="1" t="inlineStr">
         <is>
           <t>Price Item 5</t>
         </is>
       </c>
-      <c r="AV1" s="1" t="inlineStr">
+      <c r="AZ1" s="1" t="inlineStr">
         <is>
           <t>Item Details 5</t>
         </is>
       </c>
-      <c r="AW1" s="1" t="inlineStr">
+      <c r="BA1" s="1" t="inlineStr">
         <is>
           <t>Ships From Item 5</t>
         </is>
       </c>
-      <c r="AX1" s="1" t="inlineStr">
+      <c r="BB1" s="1" t="inlineStr">
         <is>
           <t>Etsy POS Item Link 5</t>
         </is>
       </c>
-      <c r="AY1" s="1" t="inlineStr">
+      <c r="BC1" s="1" t="inlineStr">
         <is>
           <t>Reviews Item 5</t>
         </is>
       </c>
-      <c r="AZ1" s="1" t="inlineStr">
+      <c r="BD1" s="1" t="inlineStr">
+        <is>
+          <t>Total Items Left in Inventory Item 5</t>
+        </is>
+      </c>
+      <c r="BE1" s="1" t="inlineStr">
         <is>
           <t>Item Sold 6 (with Reviews)</t>
         </is>
       </c>
-      <c r="BA1" s="1" t="inlineStr">
+      <c r="BF1" s="1" t="inlineStr">
         <is>
           <t>Title Item 6</t>
         </is>
       </c>
-      <c r="BB1" s="1" t="inlineStr">
+      <c r="BG1" s="1" t="inlineStr">
         <is>
           <t>Description Item 6</t>
         </is>
       </c>
-      <c r="BC1" s="1" t="inlineStr">
+      <c r="BH1" s="1" t="inlineStr">
         <is>
           <t>Price Item 6</t>
         </is>
       </c>
-      <c r="BD1" s="1" t="inlineStr">
+      <c r="BI1" s="1" t="inlineStr">
         <is>
           <t>Item Details 6</t>
         </is>
       </c>
-      <c r="BE1" s="1" t="inlineStr">
+      <c r="BJ1" s="1" t="inlineStr">
         <is>
           <t>Ships From Item 6</t>
         </is>
       </c>
-      <c r="BF1" s="1" t="inlineStr">
+      <c r="BK1" s="1" t="inlineStr">
         <is>
           <t>Etsy POS Item Link 6</t>
         </is>
       </c>
-      <c r="BG1" s="1" t="inlineStr">
+      <c r="BL1" s="1" t="inlineStr">
         <is>
           <t>Reviews Item 6</t>
         </is>
       </c>
-      <c r="BH1" s="1" t="inlineStr">
+      <c r="BM1" s="1" t="inlineStr">
+        <is>
+          <t>Total Items Left in Inventory Item 6</t>
+        </is>
+      </c>
+      <c r="BN1" s="1" t="inlineStr">
         <is>
           <t>Item No Reviews 1</t>
         </is>
       </c>
-      <c r="BI1" s="1" t="inlineStr">
+      <c r="BO1" s="1" t="inlineStr">
         <is>
           <t>Title Item 7</t>
         </is>
       </c>
-      <c r="BJ1" s="1" t="inlineStr">
+      <c r="BP1" s="1" t="inlineStr">
         <is>
           <t>Description Item 7</t>
         </is>
       </c>
-      <c r="BK1" s="1" t="inlineStr">
+      <c r="BQ1" s="1" t="inlineStr">
         <is>
           <t>Price Item 7</t>
         </is>
       </c>
-      <c r="BL1" s="1" t="inlineStr">
+      <c r="BR1" s="1" t="inlineStr">
         <is>
           <t>Item Details 7</t>
         </is>
       </c>
-      <c r="BM1" s="1" t="inlineStr">
+      <c r="BS1" s="1" t="inlineStr">
         <is>
           <t>Ships From Item 7</t>
         </is>
       </c>
-      <c r="BN1" s="1" t="inlineStr">
+      <c r="BT1" s="1" t="inlineStr">
         <is>
           <t>Etsy POS Item Link 7</t>
         </is>
       </c>
-      <c r="BO1" s="1" t="inlineStr">
+      <c r="BU1" s="1" t="inlineStr">
         <is>
           <t>Item No Reviews 2</t>
         </is>
       </c>
-      <c r="BP1" s="1" t="inlineStr">
+      <c r="BV1" s="1" t="inlineStr">
         <is>
           <t>Title Item 8</t>
         </is>
       </c>
-      <c r="BQ1" s="1" t="inlineStr">
+      <c r="BW1" s="1" t="inlineStr">
         <is>
           <t>Description Item 8</t>
         </is>
       </c>
-      <c r="BR1" s="1" t="inlineStr">
+      <c r="BX1" s="1" t="inlineStr">
         <is>
           <t>Price Item 8</t>
         </is>
       </c>
-      <c r="BS1" s="1" t="inlineStr">
+      <c r="BY1" s="1" t="inlineStr">
         <is>
           <t>Item Details 8</t>
         </is>
       </c>
-      <c r="BT1" s="1" t="inlineStr">
+      <c r="BZ1" s="1" t="inlineStr">
         <is>
           <t>Ships From Item 8</t>
         </is>
       </c>
-      <c r="BU1" s="1" t="inlineStr">
+      <c r="CA1" s="1" t="inlineStr">
         <is>
           <t>Etsy POS Item Link 8</t>
         </is>
       </c>
-      <c r="BV1" s="1" t="inlineStr">
+      <c r="CB1" s="1" t="inlineStr">
         <is>
           <t>Item No Reviews 3</t>
         </is>
       </c>
-      <c r="BW1" s="1" t="inlineStr">
+      <c r="CC1" s="1" t="inlineStr">
         <is>
           <t>Title Item 9</t>
         </is>
       </c>
-      <c r="BX1" s="1" t="inlineStr">
+      <c r="CD1" s="1" t="inlineStr">
         <is>
           <t>Description Item 9</t>
         </is>
       </c>
-      <c r="BY1" s="1" t="inlineStr">
+      <c r="CE1" s="1" t="inlineStr">
         <is>
           <t>Price Item 9</t>
         </is>
       </c>
-      <c r="BZ1" s="1" t="inlineStr">
+      <c r="CF1" s="1" t="inlineStr">
         <is>
           <t>Item Details 9</t>
         </is>
       </c>
-      <c r="CA1" s="1" t="inlineStr">
+      <c r="CG1" s="1" t="inlineStr">
         <is>
           <t>Ships From Item 9</t>
         </is>
       </c>
-      <c r="CB1" s="1" t="inlineStr">
+      <c r="CH1" s="1" t="inlineStr">
         <is>
           <t>Etsy POS Item Link 9</t>
         </is>
       </c>
-      <c r="CC1" s="1" t="inlineStr">
+      <c r="CI1" s="1" t="inlineStr">
         <is>
           <t>Social Media Platform 1 Link</t>
         </is>
       </c>
-      <c r="CD1" s="1" t="inlineStr">
+      <c r="CJ1" s="1" t="inlineStr">
         <is>
           <t>Profile Name Platform 1</t>
         </is>
       </c>
-      <c r="CE1" s="1" t="inlineStr">
+      <c r="CK1" s="1" t="inlineStr">
         <is>
           <t>Number of Followers Platform 1</t>
         </is>
       </c>
-      <c r="CF1" s="1" t="inlineStr">
+      <c r="CL1" s="1" t="inlineStr">
         <is>
           <t>Number Following Platform 1</t>
         </is>
       </c>
-      <c r="CG1" s="1" t="inlineStr">
+      <c r="CM1" s="1" t="inlineStr">
         <is>
           <t>Number of Overall Posts Platform 1</t>
         </is>
       </c>
-      <c r="CH1" s="1" t="inlineStr">
+      <c r="CN1" s="1" t="inlineStr">
         <is>
           <t>Number of Posts in Last Month Platform 1</t>
         </is>
       </c>
-      <c r="CI1" s="1" t="inlineStr">
+      <c r="CO1" s="1" t="inlineStr">
         <is>
           <t>Number of Posts in Last Week Platform 1</t>
         </is>
       </c>
-      <c r="CJ1" s="1" t="inlineStr">
+      <c r="CP1" s="1" t="inlineStr">
         <is>
           <t>Social Media Platform 2 Link</t>
         </is>
       </c>
-      <c r="CK1" s="1" t="inlineStr">
+      <c r="CQ1" s="1" t="inlineStr">
         <is>
           <t>Profile Name Platform 2</t>
         </is>
       </c>
-      <c r="CL1" s="1" t="inlineStr">
+      <c r="CR1" s="1" t="inlineStr">
         <is>
           <t>Number of Followers Platform 2</t>
         </is>
       </c>
-      <c r="CM1" s="1" t="inlineStr">
+      <c r="CS1" s="1" t="inlineStr">
         <is>
           <t>Number Following Platform 2</t>
         </is>
       </c>
-      <c r="CN1" s="1" t="inlineStr">
+      <c r="CT1" s="1" t="inlineStr">
         <is>
           <t>Number of Overall Posts Platform 2</t>
         </is>
       </c>
-      <c r="CO1" s="1" t="inlineStr">
+      <c r="CU1" s="1" t="inlineStr">
         <is>
           <t>Number of Posts in Last Month Platform 2</t>
         </is>
       </c>
-      <c r="CP1" s="1" t="inlineStr">
+      <c r="CV1" s="1" t="inlineStr">
         <is>
           <t>Number of Posts in Last Week Platform 2</t>
         </is>
       </c>
-      <c r="CQ1" s="1" t="inlineStr">
+      <c r="CW1" s="1" t="inlineStr">
         <is>
           <t>Social Media Platform 3 Link</t>
         </is>
       </c>
-      <c r="CR1" s="1" t="inlineStr">
+      <c r="CX1" s="1" t="inlineStr">
         <is>
           <t>Profile Name Platform 3</t>
         </is>
       </c>
-      <c r="CS1" s="1" t="inlineStr">
+      <c r="CY1" s="1" t="inlineStr">
         <is>
           <t>Number of Followers Platform 3</t>
         </is>
       </c>
-      <c r="CT1" s="1" t="inlineStr">
+      <c r="CZ1" s="1" t="inlineStr">
         <is>
           <t>Number Following Platform 3</t>
         </is>
       </c>
-      <c r="CU1" s="1" t="inlineStr">
+      <c r="DA1" s="1" t="inlineStr">
         <is>
           <t>Number of Overall Posts Platform 3</t>
         </is>
       </c>
-      <c r="CV1" s="1" t="inlineStr">
+      <c r="DB1" s="1" t="inlineStr">
         <is>
           <t>Number of Posts in Last Month Platform 3</t>
         </is>
       </c>
-      <c r="CW1" s="1" t="inlineStr">
+      <c r="DC1" s="1" t="inlineStr">
         <is>
           <t>Number of Posts in Last Week Platform 3</t>
         </is>
       </c>
-      <c r="CX1" s="1" t="inlineStr">
+      <c r="DD1" s="1" t="inlineStr">
         <is>
           <t>Meta Ad 1 Title</t>
         </is>
       </c>
-      <c r="CY1" s="1" t="inlineStr">
+      <c r="DE1" s="1" t="inlineStr">
         <is>
           <t>Meta Ad 1 Description</t>
         </is>
       </c>
-      <c r="CZ1" s="1" t="inlineStr">
+      <c r="DF1" s="1" t="inlineStr">
         <is>
           <t>Meta Ad 1 Details</t>
         </is>
       </c>
-      <c r="DA1" s="1" t="inlineStr">
+      <c r="DG1" s="1" t="inlineStr">
         <is>
           <t>Meta Ad 1 Advertiser Name</t>
         </is>
       </c>
-      <c r="DB1" s="1" t="inlineStr">
+      <c r="DH1" s="1" t="inlineStr">
         <is>
           <t>Meta Ad 1 Posting Date</t>
         </is>
       </c>
-      <c r="DC1" s="1" t="inlineStr">
+      <c r="DI1" s="1" t="inlineStr">
         <is>
           <t>Meta Ad 1 ChatGPT Visual Analysis</t>
         </is>
       </c>
-      <c r="DD1" s="1" t="inlineStr">
+      <c r="DJ1" s="1" t="inlineStr">
         <is>
           <t>Meta Ad 1 Video Transcript</t>
         </is>
       </c>
-      <c r="DE1" s="1" t="inlineStr">
+      <c r="DK1" s="1" t="inlineStr">
         <is>
           <t>Meta Ad 2 Title</t>
         </is>
       </c>
-      <c r="DF1" s="1" t="inlineStr">
+      <c r="DL1" s="1" t="inlineStr">
         <is>
           <t>Meta Ad 2 Description</t>
         </is>
       </c>
-      <c r="DG1" s="1" t="inlineStr">
+      <c r="DM1" s="1" t="inlineStr">
         <is>
           <t>Meta Ad 2 Details</t>
         </is>
       </c>
-      <c r="DH1" s="1" t="inlineStr">
+      <c r="DN1" s="1" t="inlineStr">
         <is>
           <t>Meta Ad 2 Advertiser Name</t>
         </is>
       </c>
-      <c r="DI1" s="1" t="inlineStr">
+      <c r="DO1" s="1" t="inlineStr">
         <is>
           <t>Meta Ad 2 Posting Date</t>
         </is>
       </c>
-      <c r="DJ1" s="1" t="inlineStr">
+      <c r="DP1" s="1" t="inlineStr">
         <is>
           <t>Meta Ad 2 ChatGPT Visual Analysis</t>
         </is>
       </c>
-      <c r="DK1" s="1" t="inlineStr">
+      <c r="DQ1" s="1" t="inlineStr">
         <is>
           <t>Meta Ad 2 Video Transcript</t>
         </is>
       </c>
-      <c r="DL1" s="1" t="inlineStr">
+      <c r="DR1" s="1" t="inlineStr">
         <is>
           <t>Meta Ad 3 Title</t>
         </is>
       </c>
-      <c r="DM1" s="1" t="inlineStr">
+      <c r="DS1" s="1" t="inlineStr">
         <is>
           <t>Meta Ad 3 Description</t>
         </is>
       </c>
-      <c r="DN1" s="1" t="inlineStr">
+      <c r="DT1" s="1" t="inlineStr">
         <is>
           <t>Meta Ad 3 Details</t>
         </is>
       </c>
-      <c r="DO1" s="1" t="inlineStr">
+      <c r="DU1" s="1" t="inlineStr">
         <is>
           <t>Meta Ad 3 Advertiser Name</t>
         </is>
       </c>
-      <c r="DP1" s="1" t="inlineStr">
+      <c r="DV1" s="1" t="inlineStr">
         <is>
           <t>Meta Ad 3 Posting Date</t>
         </is>
       </c>
-      <c r="DQ1" s="1" t="inlineStr">
+      <c r="DW1" s="1" t="inlineStr">
         <is>
           <t>Meta Ad 3 ChatGPT Visual Analysis</t>
         </is>
       </c>
-      <c r="DR1" s="1" t="inlineStr">
+      <c r="DX1" s="1" t="inlineStr">
         <is>
           <t>Meta Ad 3 Video Transcript</t>
+        </is>
+      </c>
+      <c r="DY1" s="1" t="inlineStr">
+        <is>
+          <t>Total Number of Items in Carts (Platform-Wide)</t>
+        </is>
+      </c>
+      <c r="DZ1" s="1" t="inlineStr">
+        <is>
+          <t>Total Number of Shares (Last 3 Months)</t>
+        </is>
+      </c>
+      <c r="EA1" s="1" t="inlineStr">
+        <is>
+          <t>Total Number of Shares (Last 2 Months)</t>
+        </is>
+      </c>
+      <c r="EB1" s="1" t="inlineStr">
+        <is>
+          <t>Total Number of Shares (Last 1 Month)</t>
+        </is>
+      </c>
+      <c r="EC1" s="1" t="inlineStr">
+        <is>
+          <t>Total Number of Shares (Last 2 Weeks)</t>
+        </is>
+      </c>
+      <c r="ED1" s="1" t="inlineStr">
+        <is>
+          <t>Total Number of Shares (Last 3 Days)</t>
+        </is>
+      </c>
+      <c r="EE1" s="1" t="inlineStr">
+        <is>
+          <t>Total Number of Impressions (Last 3 Months)</t>
+        </is>
+      </c>
+      <c r="EF1" s="1" t="inlineStr">
+        <is>
+          <t>Total Number of Impressions (Last 2 Months)</t>
+        </is>
+      </c>
+      <c r="EG1" s="1" t="inlineStr">
+        <is>
+          <t>Total Number of Impressions (Last 1 Month)</t>
+        </is>
+      </c>
+      <c r="EH1" s="1" t="inlineStr">
+        <is>
+          <t>Total Number of Impressions (Last 2 Weeks)</t>
+        </is>
+      </c>
+      <c r="EI1" s="1" t="inlineStr">
+        <is>
+          <t>Total Number of Impressions (Last 3 Days)</t>
+        </is>
+      </c>
+      <c r="EJ1" s="1" t="inlineStr">
+        <is>
+          <t>Total Number of Comments (Last 3 Months)</t>
+        </is>
+      </c>
+      <c r="EK1" s="1" t="inlineStr">
+        <is>
+          <t>Total Number of Comments (Last 2 Months)</t>
+        </is>
+      </c>
+      <c r="EL1" s="1" t="inlineStr">
+        <is>
+          <t>Total Number of Comments (Last 1 Month)</t>
+        </is>
+      </c>
+      <c r="EM1" s="1" t="inlineStr">
+        <is>
+          <t>Total Number of Comments (Last 2 Weeks)</t>
+        </is>
+      </c>
+      <c r="EN1" s="1" t="inlineStr">
+        <is>
+          <t>Total Number of Comments (Last 3 Days)</t>
+        </is>
+      </c>
+      <c r="EO1" s="1" t="inlineStr">
+        <is>
+          <t>Total Number of Likes (Last 3 Months)</t>
+        </is>
+      </c>
+      <c r="EP1" s="1" t="inlineStr">
+        <is>
+          <t>Total Number of Likes (Last 2 Months)</t>
+        </is>
+      </c>
+      <c r="EQ1" s="1" t="inlineStr">
+        <is>
+          <t>Total Number of Likes (Last 1 Month)</t>
+        </is>
+      </c>
+      <c r="ER1" s="1" t="inlineStr">
+        <is>
+          <t>Total Number of Likes (Last 2 Weeks)</t>
+        </is>
+      </c>
+      <c r="ES1" s="1" t="inlineStr">
+        <is>
+          <t>Total Number of Likes (Last 3 Days)</t>
         </is>
       </c>
     </row>

</xml_diff>